<commit_message>
Updates sample files to reflect arguments in sample_output
</commit_message>
<xml_diff>
--- a/blank_row_inserter/sample_files/result_multiplication_table.xlsx
+++ b/blank_row_inserter/sample_files/result_multiplication_table.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12210" windowWidth="28800" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="15x15 multiplication table" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="15x15 multiplication table" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -344,7 +344,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomRight" state="frozen" topLeftCell="B2" xSplit="1" ySplit="1"/>
@@ -571,602 +571,638 @@
       <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>4</v>
-      </c>
-      <c r="C6" t="n">
-        <v>8</v>
-      </c>
-      <c r="D6" t="n">
-        <v>12</v>
-      </c>
-      <c r="E6" t="n">
-        <v>16</v>
-      </c>
-      <c r="F6" t="n">
-        <v>20</v>
-      </c>
-      <c r="G6" t="n">
-        <v>24</v>
-      </c>
-      <c r="H6" t="n">
-        <v>28</v>
-      </c>
-      <c r="I6" t="n">
-        <v>32</v>
-      </c>
-      <c r="J6" t="n">
-        <v>36</v>
-      </c>
-      <c r="K6" t="n">
-        <v>40</v>
-      </c>
-      <c r="L6" t="n">
-        <v>44</v>
-      </c>
-      <c r="M6" t="n">
-        <v>48</v>
-      </c>
-      <c r="N6" t="n">
-        <v>52</v>
-      </c>
-      <c r="O6" t="n">
-        <v>56</v>
-      </c>
-      <c r="P6" t="n">
-        <v>60</v>
-      </c>
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" t="n">
-        <v>10</v>
-      </c>
-      <c r="D7" t="n">
-        <v>15</v>
-      </c>
-      <c r="E7" t="n">
-        <v>20</v>
-      </c>
-      <c r="F7" t="n">
-        <v>25</v>
-      </c>
-      <c r="G7" t="n">
-        <v>30</v>
-      </c>
-      <c r="H7" t="n">
-        <v>35</v>
-      </c>
-      <c r="I7" t="n">
-        <v>40</v>
-      </c>
-      <c r="J7" t="n">
-        <v>45</v>
-      </c>
-      <c r="K7" t="n">
-        <v>50</v>
-      </c>
-      <c r="L7" t="n">
-        <v>55</v>
-      </c>
-      <c r="M7" t="n">
-        <v>60</v>
-      </c>
-      <c r="N7" t="n">
-        <v>65</v>
-      </c>
-      <c r="O7" t="n">
-        <v>70</v>
-      </c>
-      <c r="P7" t="n">
-        <v>75</v>
-      </c>
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C8" t="n">
+        <v>8</v>
+      </c>
+      <c r="D8" t="n">
         <v>12</v>
       </c>
-      <c r="D8" t="n">
-        <v>18</v>
-      </c>
       <c r="E8" t="n">
+        <v>16</v>
+      </c>
+      <c r="F8" t="n">
+        <v>20</v>
+      </c>
+      <c r="G8" t="n">
         <v>24</v>
       </c>
-      <c r="F8" t="n">
-        <v>30</v>
-      </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
+        <v>28</v>
+      </c>
+      <c r="I8" t="n">
+        <v>32</v>
+      </c>
+      <c r="J8" t="n">
         <v>36</v>
       </c>
-      <c r="H8" t="n">
-        <v>42</v>
-      </c>
-      <c r="I8" t="n">
+      <c r="K8" t="n">
+        <v>40</v>
+      </c>
+      <c r="L8" t="n">
+        <v>44</v>
+      </c>
+      <c r="M8" t="n">
         <v>48</v>
       </c>
-      <c r="J8" t="n">
-        <v>54</v>
-      </c>
-      <c r="K8" t="n">
+      <c r="N8" t="n">
+        <v>52</v>
+      </c>
+      <c r="O8" t="n">
+        <v>56</v>
+      </c>
+      <c r="P8" t="n">
         <v>60</v>
-      </c>
-      <c r="L8" t="n">
-        <v>66</v>
-      </c>
-      <c r="M8" t="n">
-        <v>72</v>
-      </c>
-      <c r="N8" t="n">
-        <v>78</v>
-      </c>
-      <c r="O8" t="n">
-        <v>84</v>
-      </c>
-      <c r="P8" t="n">
-        <v>90</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B9" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E9" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F9" t="n">
+        <v>25</v>
+      </c>
+      <c r="G9" t="n">
+        <v>30</v>
+      </c>
+      <c r="H9" t="n">
         <v>35</v>
       </c>
-      <c r="G9" t="n">
-        <v>42</v>
-      </c>
-      <c r="H9" t="n">
-        <v>49</v>
-      </c>
       <c r="I9" t="n">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="J9" t="n">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="K9" t="n">
+        <v>50</v>
+      </c>
+      <c r="L9" t="n">
+        <v>55</v>
+      </c>
+      <c r="M9" t="n">
+        <v>60</v>
+      </c>
+      <c r="N9" t="n">
+        <v>65</v>
+      </c>
+      <c r="O9" t="n">
         <v>70</v>
       </c>
-      <c r="L9" t="n">
-        <v>77</v>
-      </c>
-      <c r="M9" t="n">
-        <v>84</v>
-      </c>
-      <c r="N9" t="n">
-        <v>91</v>
-      </c>
-      <c r="O9" t="n">
-        <v>98</v>
-      </c>
       <c r="P9" t="n">
-        <v>105</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D10" t="n">
+        <v>18</v>
+      </c>
+      <c r="E10" t="n">
         <v>24</v>
       </c>
-      <c r="E10" t="n">
-        <v>32</v>
-      </c>
       <c r="F10" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G10" t="n">
+        <v>36</v>
+      </c>
+      <c r="H10" t="n">
+        <v>42</v>
+      </c>
+      <c r="I10" t="n">
         <v>48</v>
       </c>
-      <c r="H10" t="n">
-        <v>56</v>
-      </c>
-      <c r="I10" t="n">
-        <v>64</v>
-      </c>
       <c r="J10" t="n">
+        <v>54</v>
+      </c>
+      <c r="K10" t="n">
+        <v>60</v>
+      </c>
+      <c r="L10" t="n">
+        <v>66</v>
+      </c>
+      <c r="M10" t="n">
         <v>72</v>
       </c>
-      <c r="K10" t="n">
-        <v>80</v>
-      </c>
-      <c r="L10" t="n">
-        <v>88</v>
-      </c>
-      <c r="M10" t="n">
-        <v>96</v>
-      </c>
       <c r="N10" t="n">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="O10" t="n">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="P10" t="n">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C11" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D11" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E11" t="n">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F11" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G11" t="n">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="H11" t="n">
+        <v>49</v>
+      </c>
+      <c r="I11" t="n">
+        <v>56</v>
+      </c>
+      <c r="J11" t="n">
         <v>63</v>
       </c>
-      <c r="I11" t="n">
-        <v>72</v>
-      </c>
-      <c r="J11" t="n">
-        <v>81</v>
-      </c>
       <c r="K11" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="L11" t="n">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="M11" t="n">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="N11" t="n">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="O11" t="n">
-        <v>126</v>
+        <v>98</v>
       </c>
       <c r="P11" t="n">
-        <v>135</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D12" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E12" t="n">
+        <v>32</v>
+      </c>
+      <c r="F12" t="n">
         <v>40</v>
       </c>
-      <c r="F12" t="n">
-        <v>50</v>
-      </c>
       <c r="G12" t="n">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="H12" t="n">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="I12" t="n">
+        <v>64</v>
+      </c>
+      <c r="J12" t="n">
+        <v>72</v>
+      </c>
+      <c r="K12" t="n">
         <v>80</v>
       </c>
-      <c r="J12" t="n">
-        <v>90</v>
-      </c>
-      <c r="K12" t="n">
-        <v>100</v>
-      </c>
       <c r="L12" t="n">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="M12" t="n">
+        <v>96</v>
+      </c>
+      <c r="N12" t="n">
+        <v>104</v>
+      </c>
+      <c r="O12" t="n">
+        <v>112</v>
+      </c>
+      <c r="P12" t="n">
         <v>120</v>
-      </c>
-      <c r="N12" t="n">
-        <v>130</v>
-      </c>
-      <c r="O12" t="n">
-        <v>140</v>
-      </c>
-      <c r="P12" t="n">
-        <v>150</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D13" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E13" t="n">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F13" t="n">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G13" t="n">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="H13" t="n">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="I13" t="n">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="J13" t="n">
+        <v>81</v>
+      </c>
+      <c r="K13" t="n">
+        <v>90</v>
+      </c>
+      <c r="L13" t="n">
         <v>99</v>
       </c>
-      <c r="K13" t="n">
-        <v>110</v>
-      </c>
-      <c r="L13" t="n">
-        <v>121</v>
-      </c>
       <c r="M13" t="n">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="N13" t="n">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="O13" t="n">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="P13" t="n">
-        <v>165</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D14" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E14" t="n">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F14" t="n">
+        <v>50</v>
+      </c>
+      <c r="G14" t="n">
         <v>60</v>
       </c>
-      <c r="G14" t="n">
-        <v>72</v>
-      </c>
       <c r="H14" t="n">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="I14" t="n">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="J14" t="n">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="K14" t="n">
+        <v>100</v>
+      </c>
+      <c r="L14" t="n">
+        <v>110</v>
+      </c>
+      <c r="M14" t="n">
         <v>120</v>
       </c>
-      <c r="L14" t="n">
-        <v>132</v>
-      </c>
-      <c r="M14" t="n">
-        <v>144</v>
-      </c>
       <c r="N14" t="n">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="O14" t="n">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="P14" t="n">
-        <v>180</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D15" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E15" t="n">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F15" t="n">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="G15" t="n">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="H15" t="n">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="I15" t="n">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="J15" t="n">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="K15" t="n">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="L15" t="n">
+        <v>121</v>
+      </c>
+      <c r="M15" t="n">
+        <v>132</v>
+      </c>
+      <c r="N15" t="n">
         <v>143</v>
       </c>
-      <c r="M15" t="n">
-        <v>156</v>
-      </c>
-      <c r="N15" t="n">
-        <v>169</v>
-      </c>
       <c r="O15" t="n">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="P15" t="n">
-        <v>195</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C16" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D16" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E16" t="n">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F16" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G16" t="n">
+        <v>72</v>
+      </c>
+      <c r="H16" t="n">
         <v>84</v>
       </c>
-      <c r="H16" t="n">
-        <v>98</v>
-      </c>
       <c r="I16" t="n">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="J16" t="n">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="K16" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="L16" t="n">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="M16" t="n">
+        <v>144</v>
+      </c>
+      <c r="N16" t="n">
+        <v>156</v>
+      </c>
+      <c r="O16" t="n">
         <v>168</v>
       </c>
-      <c r="N16" t="n">
-        <v>182</v>
-      </c>
-      <c r="O16" t="n">
-        <v>196</v>
-      </c>
       <c r="P16" t="n">
-        <v>210</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
+        <v>13</v>
+      </c>
+      <c r="B17" t="n">
+        <v>13</v>
+      </c>
+      <c r="C17" t="n">
+        <v>26</v>
+      </c>
+      <c r="D17" t="n">
+        <v>39</v>
+      </c>
+      <c r="E17" t="n">
+        <v>52</v>
+      </c>
+      <c r="F17" t="n">
+        <v>65</v>
+      </c>
+      <c r="G17" t="n">
+        <v>78</v>
+      </c>
+      <c r="H17" t="n">
+        <v>91</v>
+      </c>
+      <c r="I17" t="n">
+        <v>104</v>
+      </c>
+      <c r="J17" t="n">
+        <v>117</v>
+      </c>
+      <c r="K17" t="n">
+        <v>130</v>
+      </c>
+      <c r="L17" t="n">
+        <v>143</v>
+      </c>
+      <c r="M17" t="n">
+        <v>156</v>
+      </c>
+      <c r="N17" t="n">
+        <v>169</v>
+      </c>
+      <c r="O17" t="n">
+        <v>182</v>
+      </c>
+      <c r="P17" t="n">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>14</v>
+      </c>
+      <c r="B18" t="n">
+        <v>14</v>
+      </c>
+      <c r="C18" t="n">
+        <v>28</v>
+      </c>
+      <c r="D18" t="n">
+        <v>42</v>
+      </c>
+      <c r="E18" t="n">
+        <v>56</v>
+      </c>
+      <c r="F18" t="n">
+        <v>70</v>
+      </c>
+      <c r="G18" t="n">
+        <v>84</v>
+      </c>
+      <c r="H18" t="n">
+        <v>98</v>
+      </c>
+      <c r="I18" t="n">
+        <v>112</v>
+      </c>
+      <c r="J18" t="n">
+        <v>126</v>
+      </c>
+      <c r="K18" t="n">
+        <v>140</v>
+      </c>
+      <c r="L18" t="n">
+        <v>154</v>
+      </c>
+      <c r="M18" t="n">
+        <v>168</v>
+      </c>
+      <c r="N18" t="n">
+        <v>182</v>
+      </c>
+      <c r="O18" t="n">
+        <v>196</v>
+      </c>
+      <c r="P18" t="n">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B19" t="n">
         <v>15</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C19" t="n">
         <v>30</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D19" t="n">
         <v>45</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E19" t="n">
         <v>60</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F19" t="n">
         <v>75</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G19" t="n">
         <v>90</v>
       </c>
-      <c r="H17" t="n">
+      <c r="H19" t="n">
         <v>105</v>
       </c>
-      <c r="I17" t="n">
+      <c r="I19" t="n">
         <v>120</v>
       </c>
-      <c r="J17" t="n">
+      <c r="J19" t="n">
         <v>135</v>
       </c>
-      <c r="K17" t="n">
+      <c r="K19" t="n">
         <v>150</v>
       </c>
-      <c r="L17" t="n">
+      <c r="L19" t="n">
         <v>165</v>
       </c>
-      <c r="M17" t="n">
+      <c r="M19" t="n">
         <v>180</v>
       </c>
-      <c r="N17" t="n">
+      <c r="N19" t="n">
         <v>195</v>
       </c>
-      <c r="O17" t="n">
+      <c r="O19" t="n">
         <v>210</v>
       </c>
-      <c r="P17" t="n">
+      <c r="P19" t="n">
         <v>225</v>
       </c>
     </row>

</xml_diff>